<commit_message>
support inport lqsutra info.
</commit_message>
<xml_diff>
--- a/test/乾隆大藏经详目20170713_test_simple.xlsx
+++ b/test/乾隆大藏经详目20170713_test_simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24460" windowHeight="15360"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="23580" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,103 +21,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+  <si>
+    <t>series</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_volume</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_page</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_volume</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_page</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL0003</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>remark</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V1_P2</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V2_P34</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V2_P89</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V1</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL0001_R1</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL0003_R1</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>重刊藏經序（2-3页）；貞觀三藏聖教序（4-5页）；永徽三藏聖教記（6-7页）；正統御製大藏經序（8-9页）；萬曆御製新刋續入藏經序（10-11页）；萬曆御製聖母印施佛藏經序（12-13页）；聖母印施佛藏經讚（14-16页）；大般若經初會序（17-17页）</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V1</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V1_P27</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL0001</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL_V2</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>sutra__name</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>sutra</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>sutra__lqsutra</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>sutra__lqsutra__name</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>LQ001</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>LQ003</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>LQ大般若波羅蜜多經</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
+  <si>
+    <t>LQ大清三藏聖教目錄</t>
+    <phoneticPr fontId="27" type="noConversion"/>
+  </si>
   <si>
     <t>大清三藏聖教目錄</t>
+    <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
     <t>大般若波羅蜜多經</t>
-  </si>
-  <si>
-    <t>series</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>sutra</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>start_volume</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>start_page</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>end_volume</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>end_page</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>code</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL0003</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>remark</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V1_P2</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V2_P34</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V2_P89</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V1</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL0001_R1</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL0003_R1</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>重刊藏經序（2-3页）；貞觀三藏聖教序（4-5页）；永徽三藏聖教記（6-7页）；正統御製大藏經序（8-9页）；萬曆御製新刋續入藏經序（10-11页）；萬曆御製聖母印施佛藏經序（12-13页）；聖母印施佛藏經讚（14-16页）；大般若經初會序（17-17页）</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V1</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V1_P27</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL0001</t>
-    <phoneticPr fontId="27" type="noConversion"/>
-  </si>
-  <si>
-    <t>QL_V2</t>
     <phoneticPr fontId="27" type="noConversion"/>
   </si>
 </sst>
@@ -597,7 +623,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -823,6 +849,8 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -880,7 +908,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="99">
     <cellStyle name="20% - 强调文字颜色 1 2" xfId="1"/>
     <cellStyle name="20% - 强调文字颜色 2 2" xfId="18"/>
     <cellStyle name="20% - 强调文字颜色 3 2" xfId="20"/>
@@ -946,6 +974,7 @@
     <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
@@ -954,6 +983,7 @@
     <cellStyle name="访问过的超链接" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="好 2" xfId="67"/>
     <cellStyle name="汇总 2" xfId="68"/>
     <cellStyle name="计算 2" xfId="3"/>
@@ -1276,109 +1306,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="I1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="K1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="18">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="18">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="18">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="27" type="noConversion"/>

</xml_diff>